<commit_message>
add styling, correct data
</commit_message>
<xml_diff>
--- a/BIMetadata.xlsx
+++ b/BIMetadata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>xx Main Version xx</t>
   </si>
@@ -334,130 +334,115 @@
     <t>Release</t>
   </si>
   <si>
+    <t>DLM - Another Reminder v1 (Full).wav</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>DL Music</t>
+  </si>
+  <si>
+    <t>Another Reminder v4 (No Risers)</t>
+  </si>
+  <si>
+    <t>DLM - Another Reminder v4 (No Risers).wav</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Jazz, Smooth Jazz Vol.42</t>
+  </si>
+  <si>
+    <t>DLM-BI-176-R42</t>
+  </si>
+  <si>
+    <t>Jazz (Smooth)</t>
+  </si>
+  <si>
+    <t>2020422</t>
+  </si>
+  <si>
+    <t>Hal  Stephens </t>
+  </si>
+  <si>
+    <t>Derek Luff</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>DL Music</t>
-  </si>
-  <si>
-    <t>Another Chance v1 (Full)</t>
-  </si>
-  <si>
-    <t>DLM - Another Chance v1 (Full).mp3</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Bumpers - Transitions, Driving Vol.40</t>
-  </si>
-  <si>
-    <t>DLM-BI-103-R40</t>
-  </si>
-  <si>
-    <t>Stingers (Driving)</t>
-  </si>
-  <si>
-    <t>2020401</t>
-  </si>
-  <si>
-    <t>Joyion Cne Timmons </t>
-  </si>
-  <si>
-    <t>Derek Luff</t>
-  </si>
-  <si>
     <t>Songs</t>
   </si>
   <si>
-    <t>08-19-2020</t>
+    <t>08-20-2020</t>
   </si>
   <si>
     <t>70's,80's,Acoustic</t>
   </si>
   <si>
-    <t>Driving</t>
+    <t>Smooth Jazz</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
+    <t>US-RRD-20-00002</t>
+  </si>
+  <si>
+    <t>ASCAP</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Original Publisher</t>
+  </si>
+  <si>
+    <t>Hal</t>
+  </si>
+  <si>
+    <t>Stephens</t>
+  </si>
+  <si>
+    <t>Composer, Writer</t>
+  </si>
+  <si>
+    <t>Accordion,Acoustic Guitar,Alto Sax</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>Nothing In This World v1 (Full)</t>
+  </si>
+  <si>
+    <t>DLM - Nothing In This World v1 (Full).wav</t>
+  </si>
+  <si>
+    <t>N/A, N/A Vol.42</t>
+  </si>
+  <si>
+    <t>DLM-BI-NaN-R42</t>
+  </si>
+  <si>
+    <t>2020423</t>
+  </si>
+  <si>
+    <t>US-RRD-20-00003</t>
+  </si>
+  <si>
+    <t>Another Reminder v1 (Full)</t>
+  </si>
+  <si>
+    <t>2020421</t>
+  </si>
+  <si>
     <t>US-RRD-20-00001</t>
-  </si>
-  <si>
-    <t>ASCAP</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Original Publisher</t>
-  </si>
-  <si>
-    <t>Joyion</t>
-  </si>
-  <si>
-    <t>Timmons</t>
-  </si>
-  <si>
-    <t>Composer, Writer</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>Accordion,Acoustic Guitar,Alto Sax</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>Reflection Pool v2 (No BsNDrms)</t>
-  </si>
-  <si>
-    <t>DLM - Reflection Pool v2 (No BsNDrms).mp3</t>
-  </si>
-  <si>
-    <t>N/A, N/A Vol.40</t>
-  </si>
-  <si>
-    <t>DLM-BI-NaN-R40</t>
-  </si>
-  <si>
-    <t>2020403</t>
-  </si>
-  <si>
-    <t>US-RRD-20-00003</t>
-  </si>
-  <si>
-    <t>Cornbread</t>
-  </si>
-  <si>
-    <t>DLM - Cornbread.mp3</t>
-  </si>
-  <si>
-    <t>2020402</t>
-  </si>
-  <si>
-    <t>US-RRD-20-00002</t>
-  </si>
-  <si>
-    <t>Reflection Pool v3 (No PadNFlute)</t>
-  </si>
-  <si>
-    <t>DLM - Reflection Pool v3 (No PadNFlute).mp3</t>
-  </si>
-  <si>
-    <t>2020404</t>
-  </si>
-  <si>
-    <t>US-RRD-20-00004</t>
   </si>
 </sst>
 </file>
@@ -497,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DC5"/>
+  <dimension ref="A1:DC4"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -876,25 +861,25 @@
         <v>115</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S2" s="0" t="s">
         <v>112</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>112</v>
@@ -903,13 +888,13 @@
         <v>112</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA2" s="0" t="s">
         <v>112</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AC2" s="0" t="s">
         <v>112</v>
@@ -918,49 +903,49 @@
         <v>118</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AF2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AN2" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AO2" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AP2" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="AI2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AK2" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP2" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="AQ2" s="0" t="s">
         <v>112</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AT2" s="0" t="s">
         <v>112</v>
@@ -981,7 +966,7 @@
         <v>112</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BA2" s="0" t="s">
         <v>112</v>
@@ -1005,7 +990,7 @@
         <v>112</v>
       </c>
       <c r="BH2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BI2" s="0" t="s">
         <v>112</v>
@@ -1026,7 +1011,7 @@
         <v>112</v>
       </c>
       <c r="BO2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BP2" s="0" t="s">
         <v>112</v>
@@ -1050,7 +1035,7 @@
         <v>112</v>
       </c>
       <c r="BW2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BX2" s="0" t="s">
         <v>112</v>
@@ -1071,7 +1056,7 @@
         <v>112</v>
       </c>
       <c r="CD2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CE2" s="0" t="s">
         <v>112</v>
@@ -1095,7 +1080,7 @@
         <v>112</v>
       </c>
       <c r="CL2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CM2" s="0" t="s">
         <v>112</v>
@@ -1116,7 +1101,7 @@
         <v>112</v>
       </c>
       <c r="CS2" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CT2" s="0" t="s">
         <v>112</v>
@@ -1151,7 +1136,7 @@
     </row>
     <row r="3" spans="1:107">
       <c r="A3" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>108</v>
@@ -1178,10 +1163,10 @@
         <v>138</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>139</v>
@@ -1196,29 +1181,29 @@
         <v>112</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="R3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="S3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="X3" s="0" t="s">
         <v>112</v>
       </c>
@@ -1226,7 +1211,7 @@
         <v>112</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA3" s="0" t="s">
         <v>112</v>
@@ -1238,7 +1223,7 @@
         <v>112</v>
       </c>
       <c r="AD3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AE3" s="0" t="s">
         <v>112</v>
@@ -1259,7 +1244,7 @@
         <v>112</v>
       </c>
       <c r="AK3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AL3" s="0" t="s">
         <v>112</v>
@@ -1283,7 +1268,7 @@
         <v>112</v>
       </c>
       <c r="AS3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AT3" s="0" t="s">
         <v>112</v>
@@ -1304,7 +1289,7 @@
         <v>112</v>
       </c>
       <c r="AZ3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BA3" s="0" t="s">
         <v>112</v>
@@ -1328,7 +1313,7 @@
         <v>112</v>
       </c>
       <c r="BH3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BI3" s="0" t="s">
         <v>112</v>
@@ -1349,7 +1334,7 @@
         <v>112</v>
       </c>
       <c r="BO3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BP3" s="0" t="s">
         <v>112</v>
@@ -1373,7 +1358,7 @@
         <v>112</v>
       </c>
       <c r="BW3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BX3" s="0" t="s">
         <v>112</v>
@@ -1394,7 +1379,7 @@
         <v>112</v>
       </c>
       <c r="CD3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CE3" s="0" t="s">
         <v>112</v>
@@ -1418,7 +1403,7 @@
         <v>112</v>
       </c>
       <c r="CL3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CM3" s="0" t="s">
         <v>112</v>
@@ -1439,7 +1424,7 @@
         <v>112</v>
       </c>
       <c r="CS3" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CT3" s="0" t="s">
         <v>112</v>
@@ -1474,7 +1459,7 @@
     </row>
     <row r="4" spans="1:107">
       <c r="A4" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>108</v>
@@ -1489,7 +1474,7 @@
         <v>141</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>112</v>
@@ -1501,67 +1486,67 @@
         <v>138</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="L4" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB4" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="M4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="X4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="AC4" s="0" t="s">
         <v>112</v>
       </c>
       <c r="AD4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AE4" s="0" t="s">
         <v>112</v>
@@ -1582,7 +1567,7 @@
         <v>112</v>
       </c>
       <c r="AK4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AL4" s="0" t="s">
         <v>112</v>
@@ -1606,7 +1591,7 @@
         <v>112</v>
       </c>
       <c r="AS4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="AT4" s="0" t="s">
         <v>112</v>
@@ -1627,7 +1612,7 @@
         <v>112</v>
       </c>
       <c r="AZ4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BA4" s="0" t="s">
         <v>112</v>
@@ -1651,7 +1636,7 @@
         <v>112</v>
       </c>
       <c r="BH4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BI4" s="0" t="s">
         <v>112</v>
@@ -1672,7 +1657,7 @@
         <v>112</v>
       </c>
       <c r="BO4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BP4" s="0" t="s">
         <v>112</v>
@@ -1696,7 +1681,7 @@
         <v>112</v>
       </c>
       <c r="BW4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="BX4" s="0" t="s">
         <v>112</v>
@@ -1717,7 +1702,7 @@
         <v>112</v>
       </c>
       <c r="CD4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CE4" s="0" t="s">
         <v>112</v>
@@ -1741,7 +1726,7 @@
         <v>112</v>
       </c>
       <c r="CL4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CM4" s="0" t="s">
         <v>112</v>
@@ -1762,7 +1747,7 @@
         <v>112</v>
       </c>
       <c r="CS4" s="0" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="CT4" s="0" t="s">
         <v>112</v>
@@ -1792,329 +1777,6 @@
         <v>112</v>
       </c>
       <c r="DC4" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:107">
-      <c r="A5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="U5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="X5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB5" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AH5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AK5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="AL5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AN5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AO5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AP5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AQ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AR5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AS5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="AT5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AU5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AV5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AW5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AY5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AZ5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="BA5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BB5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BC5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BD5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BE5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BF5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BG5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BH5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="BI5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BK5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BL5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BM5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BN5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BO5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="BP5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BQ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BR5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BS5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BT5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BU5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BV5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BW5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="BX5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BY5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BZ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CA5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CB5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CC5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CD5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="CE5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CF5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CG5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CH5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CI5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CJ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CK5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CL5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="CM5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CN5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CO5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CP5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CQ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CR5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CS5" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="CT5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CU5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CV5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CW5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CX5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CY5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="CZ5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="DA5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="DB5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="DC5" s="0" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>